<commit_message>
tweaking. separate pages in the xlsx for 10/12/15/17/20M ..2M seems impossible
</commit_message>
<xml_diff>
--- a/tracker/WSPRDenom-modified.xlsx
+++ b/tracker/WSPRDenom-modified.xlsx
@@ -8,7 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="10M" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="12M" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="15M" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="17M" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="20M" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="2M experimental" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="76">
   <si>
     <t xml:space="preserve">adjust for band/channel</t>
   </si>
@@ -217,6 +222,9 @@
     <t xml:space="preserve">Target symbol freqs</t>
   </si>
   <si>
+    <t xml:space="preserve">note this is the 4th freq bin</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -337,12 +345,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">trying to see, instead of 1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">556849 10M code suggest?</t>
   </si>
   <si>
     <t xml:space="preserve">554667 good for 10M with mul 34</t>
   </si>
   <si>
+    <t xml:space="preserve">Div 64 for 20M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">277333 for 20M, mul 34, div 64</t>
+  </si>
+  <si>
     <t xml:space="preserve">Div 50 for 17M</t>
   </si>
   <si>
@@ -391,7 +426,7 @@
     <t xml:space="preserve">Mult is created from </t>
   </si>
   <si>
-    <t xml:space="preserve">Num incrementer:1 normally, 3 on 17M</t>
+    <t xml:space="preserve">Num incrementer:1 on 20M, 10M, 3 on 17M, 2 on 12M, 2 on 15M</t>
   </si>
   <si>
     <t xml:space="preserve">working backwards from the output freq to pll freq</t>
@@ -415,76 +450,97 @@
     <t xml:space="preserve">keep an eye on keeping yellow absolute error small</t>
   </si>
   <si>
+    <t xml:space="preserve">start at 342139 for 4th freq bin on 10M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hans had 342028, 342029, 342030, 342031 as the Num when freq bin 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red above is the target optiimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue on left is the variable to change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plugging the new pll_denom into my code, I got slightly different pll_nums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the variable to change is unconstrained?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342030, 342031, 342032, 342033 when freq bin 1 on 10M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can eyeball for legal (0 to 1048575)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derived from Hans G0UPL qrp-labs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal seek to 0.04 and it should succeed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator calculated just using the "goal seek" function in the attached crappy 2 minute thrown-together spreadsheet, targeting 375 / 256. Approx a 200,000 fold improvement in tone spacing accuracy. Ain't that sweet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on Tools/Goal Seek, with cursor on I13 or L13 for target. Target value &lt; 0.04. Variable is $F9. If it doesn’t succeed, accept the best it got to update $F9. Int($F9) goes into the Den column, since the optimization creates a real.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980#msg18933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after hand experiments for 26Mhz tcxo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 10M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 12M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libreoffice goal seek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 15M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 17M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel similar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 20M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Div 36 for 12M</t>
+  </si>
+  <si>
     <t xml:space="preserve">start at 342138 for 4th freq bin on 10M</t>
   </si>
   <si>
-    <t xml:space="preserve">Hans had 342028, 342029, 342030, 342031 as the Num when freq bin 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red above is the target optiimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue on left is the variable to change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plugging the new pll_denom into my code, I got slightly different pll_nums</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the variable to change is unconstrained?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">342030, 342031, 342032, 342033 when freq bin 1 on 10M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">can eyeball for legal (0 to 1048575)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derived from Hans G0UPL qrp-labs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal seek to 0.04 and it should succeed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator calculated just using the "goal seek" function in the attached crappy 2 minute thrown-together spreadsheet, targeting 375 / 256. Approx a 200,000 fold improvement in tone spacing accuracy. Ain't that sweet?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click on Tools/Goal Seek, with cursor on I13 or L13 for target. Target value &lt; 0.04. Variable is $F9. If it doesn’t succeed, accept the best it got to update $F9. Int($F9) goes into the Den column, since the optimization creates a real.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980#msg18933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">after hand experiments for 26Mhz tcxo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 10M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 12M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libreoffice goal seek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 15M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 17M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel similar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 20M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7</t>
+    <t xml:space="preserve">845206 for 15M, mul 34, div 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Div 42 for 15M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2M 456174 mul 33 div 6 (26Mhz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mult. Allow real for 2M?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incremental shifts</t>
   </si>
 </sst>
 </file>
@@ -890,7 +946,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -975,38 +1031,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>18106020</v>
+        <v>28126180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>18106017.8027344</v>
+        <v>28126177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>18106019.2675781</v>
+        <v>28126179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>18106020.7324219</v>
+        <v>28126180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -1024,76 +1086,80 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>18106022.1972656</v>
+        <v>28126182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>1064960.885</v>
+        <v>554667</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="8" t="n">
-        <v>51</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,263 +1170,259 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>859065</v>
+        <v>342139</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>1048575</v>
+        <v>554667</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>905300994.206423</v>
+        <v>900037755.986925</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>18106019.8841285</v>
+        <v>28126179.8745914</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.08139408752322</v>
+        <v>2.07185704261065</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>859068</v>
+        <v>342140</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>905301068.593091</v>
+        <v>900037802.861897</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>18106021.3718618</v>
+        <v>28126181.3394343</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.48773334920406</v>
+        <v>1.46484287455678</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>0.0228895992040634</v>
+        <v>-8.7544322013855E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>22889.5992040634</v>
+        <v>-0.87544322013855</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.10428368672729</v>
+        <v>2.07185616716743</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>1264.19817661519</v>
+        <v>0.0311255626767625</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>859071</v>
+        <v>342141</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>905301142.979758</v>
+        <v>900037849.736869</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>18106022.8595952</v>
+        <v>28126182.8042772</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.48773335292935</v>
+        <v>1.46484287083149</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>-8.79168510437012E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>22889.6029293537</v>
+        <v>-0.879168510437012</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.12717328965664</v>
+        <v>2.07185528799891</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>859074</v>
+        <v>342142</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>905301217.366426</v>
+        <v>900037896.611841</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>18106024.3473285</v>
+        <v>28126184.26912</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.48773335292935</v>
+        <v>1.46484287083149</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>-8.79168510437012E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>22889.6029293537</v>
+        <v>-0.879168510437012</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.15006289258599</v>
+        <v>2.0718544088304</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="n">
-        <f aca="false">B11</f>
-        <v>26000000</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>905301000</v>
+        <v>900037760</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>18106020</v>
+        <v>28126180</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1" t="n">
-        <f aca="false">F16/B16</f>
-        <v>34.8192692307692</v>
+        <f aca="false">F16/B11</f>
+        <v>34.6168369230769</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.81926923076923</v>
+        <v>0.616836923076924</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D19" s="18" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>859065.233653845</v>
+        <v>342139.085612308</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="L27" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="L29" s="21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M29" s="21"/>
       <c r="N29" s="21"/>
@@ -1369,17 +1431,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -1387,39 +1449,39 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="I35" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="22" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -1458,4 +1520,2924 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>24926177.8027344</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>24926179.2675781</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>24926180.7324219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>24926182.1972656</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>986074</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>506026</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>986074</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>897342483.424165</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>24926180.0951157</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>2.29238131642342</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">D11+D17</f>
+        <v>506028</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>897342536.158544</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>24926181.5599596</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.46484386175871</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>1.11758708953857E-007</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>0.111758708953857</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>2.29238142818213</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>0.00448358721471331</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>506030</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>897342588.892923</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>24926183.0248034</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.46484385803342</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>1.08033418655396E-007</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>0.108033418655396</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>2.29238153621554</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>506032</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>897342641.627302</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>24926184.4896473</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.46484386175871</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>1.11758708953857E-007</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>0.111758708953857</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>2.29238164797425</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>897342480</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>24926180</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>34.5131723076923</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="17"/>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.513172307692308</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>506025.870135385</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>21096180</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>21096177.8027344</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>21096179.2675781</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>21096180.7324219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>21096182.1972656</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>845206</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>66302</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>845206</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>886039564.319231</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>21096180.1028388</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>2.30010445788503</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">D11+D17</f>
+        <v>66304</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>886039625.842694</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>21096181.5676832</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.46484435722232</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>6.07222318649292E-007</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>0.607222318649292</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>2.30010506510735</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>0.0287835178466365</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>66306</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>886039687.366157</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>21096183.0325275</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.46484435349703</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>6.0349702835083E-007</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>0.60349702835083</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>2.30010566860437</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>66308</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>886039748.88962</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>21096184.4973719</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.46484435349703</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>6.0349702835083E-007</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>0.60349702835083</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>2.3001062721014</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>886039560</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>21096180</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>34.0784446153846</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="17"/>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.0784446153846119</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>66301.8595907663</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>18106017.8027344</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>18106019.2675781</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>18106020.7324219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>18106022.1972656</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>1064960.885</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>859065</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>1048575</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>905300994.206423</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>18106019.8841285</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>2.08139408752322</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">D11+D17</f>
+        <v>859068</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>905301068.593091</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>18106021.3718618</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.48773334920406</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>0.0228895992040634</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>22889.5992040634</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>2.10428368672729</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>1264.19817661519</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>859071</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>905301142.979758</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>18106022.8595952</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.48773335292935</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>0.0228896029293537</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>22889.6029293537</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>2.12717328965664</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>859074</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>905301217.366426</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>18106024.3473285</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.48773335292935</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>0.0228896029293537</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>22889.6029293537</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>2.15006289258599</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>905301000</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>18106020</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>34.8192692307692</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="17"/>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.81926923076923</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>859065.233653845</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>14097177.8027344</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>14097179.2675781</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>14097180.7324219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>14097182.1972656</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>277333</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>194341</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>277333</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>902219490.648426</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>14097179.5413817</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>1.73864728398621</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">D11+D17</f>
+        <v>194342</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>902219584.398539</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>14097181.0062272</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.46484551392496</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>1.76392495632172E-006</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>1.76392495632172</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>1.73864904791117</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>0.125126077017989</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>194343</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>902219678.148652</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>14097182.4710727</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.46484551019967</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>1.76019966602325E-006</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>1.76019966602325</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>1.73865080811083</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>194344</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>902219771.898764</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>14097183.9359182</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.46484551019967</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>1.76019966602325E-006</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>1.76019966602325</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>1.7386525683105</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>902219520</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>14097180</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>34.7007507692308</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="17"/>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.700750769230773</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>194341.313083078</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>144885180</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>144885177.802734</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>144885179.267578</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>144885180.732422</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>144885182.197266</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>1973529.60362751</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>1048575</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>1040002479.55559</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>104000247.955559</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>-40884929.8471756</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">$D11 + D17</f>
+        <v>101</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>1040002504.35114</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>104000250.435114</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>2.47955559194088</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>1.01471184194088</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>1014711.84194088</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>-40884928.8324638</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>9756.82113932945</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>102</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>1040002529.1467</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>104000252.91467</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>2.47955557703972</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>1.01471182703972</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>1014711.82703972</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>-40884927.817752</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>103</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>1040002553.94226</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>104000255.394226</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>2.47955560684204</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>1.01471185684204</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>1014711.85684204</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>-40884926.8030401</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>1448851800</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>144885180</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>55.7250692307692</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="17"/>
+      <c r="E18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>15.7250692307692</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>16488914.4686538</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
700 mhz pll target, optimal denoms for 10/12/15/17/20M (from spreadsheet) seems good
</commit_message>
<xml_diff>
--- a/tracker/WSPRDenom-modified.xlsx
+++ b/tracker/WSPRDenom-modified.xlsx
@@ -8,12 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="10M" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="12M" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="15M" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="17M" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="20M" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="2M experimental" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="2M calced" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="10M" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="12M" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="15M" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="17M" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="20M" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="82">
   <si>
     <t xml:space="preserve">adjust for band/channel</t>
   </si>
@@ -34,6 +34,150 @@
   </si>
   <si>
     <t xml:space="preserve">shift from center?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target center-of-bin freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target symbol freqs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center of wspr passband</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denom optimization cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcxo freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mult. Allow real for 2M?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Den</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLL frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incremental shifts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inc. shift error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error*1e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">absolute symbol error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abs(error/freq) * 1e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed numerator for 2M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change the denom for shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mult is created from </t>
+  </si>
+  <si>
+    <t xml:space="preserve">num incrementer is 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working backwards from the output freq to pll freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outside approx. algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real multiplier:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractional part:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 &lt; Num &lt;= 1048575, required. Enforced now!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fractional pll freq:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep an eye on keeping yellow absolute error small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hans had 505514, 505513, 505512, 505511 for ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red above is the target optiimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue on left is the variable to change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the variable to change is unconstrained?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can eyeball for legal (0 to 1048575)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derived from Hans G0UPL qrp-labs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goal seek to 0.04 and it should succeed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator calculated just using the "goal seek" function in the attached crappy 2 minute thrown-together spreadsheet, targeting 375 / 256. Approx a 200,000 fold improvement in tone spacing accuracy. Ain't that sweet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on Tools/Goal Seek, with cursor on I13 or L13 for target. Target value &lt; 0.04. Variable is $F9. If it doesn’t succeed, accept the best it got to update $F9. Int($F9) goes into the Den column, since the optimization creates a real.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980#msg18933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after hand experiments for 26Mhz tcxo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 10M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 12M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libreoffice goal seek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 15M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 17M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel similar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denom for 20M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7</t>
   </si>
   <si>
     <r>
@@ -216,12 +360,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Target center-of-bin freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target symbol freqs</t>
-  </si>
-  <si>
     <t xml:space="preserve">note this is the 4th freq bin</t>
   </si>
   <si>
@@ -384,144 +522,33 @@
     <t xml:space="preserve">Be sure to fill first Num with reasonable</t>
   </si>
   <si>
-    <t xml:space="preserve">Denom optimization cell</t>
-  </si>
-  <si>
     <t xml:space="preserve">Div 32 for 10M</t>
   </si>
   <si>
     <t xml:space="preserve">estimate from approximation algo</t>
   </si>
   <si>
-    <t xml:space="preserve">tcxo freq</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mult</t>
   </si>
   <si>
-    <t xml:space="preserve">Num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Den</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLL frequency</t>
-  </si>
-  <si>
     <t xml:space="preserve">incremental shifts</t>
   </si>
   <si>
-    <t xml:space="preserve">inc. shift error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error*1e6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absolute symbol error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abs(error/freq) * 1e6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mult is created from </t>
-  </si>
-  <si>
     <t xml:space="preserve">Num incrementer:1 on 20M, 10M, 3 on 17M, 2 on 12M, 2 on 15M</t>
   </si>
   <si>
-    <t xml:space="preserve">working backwards from the output freq to pll freq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outside approx. algo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real multiplier:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fractional part:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 &lt; Num &lt;= 1048575, required. Enforced now!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fractional pll freq:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep an eye on keeping yellow absolute error small</t>
-  </si>
-  <si>
     <t xml:space="preserve">start at 342139 for 4th freq bin on 10M</t>
   </si>
   <si>
     <t xml:space="preserve">Hans had 342028, 342029, 342030, 342031 as the Num when freq bin 1</t>
   </si>
   <si>
-    <t xml:space="preserve">red above is the target optiimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue on left is the variable to change</t>
-  </si>
-  <si>
     <t xml:space="preserve">plugging the new pll_denom into my code, I got slightly different pll_nums</t>
   </si>
   <si>
-    <t xml:space="preserve">the variable to change is unconstrained?</t>
-  </si>
-  <si>
     <t xml:space="preserve">342030, 342031, 342032, 342033 when freq bin 1 on 10M</t>
   </si>
   <si>
-    <t xml:space="preserve">can eyeball for legal (0 to 1048575)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derived from Hans G0UPL qrp-labs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">goal seek to 0.04 and it should succeed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator calculated just using the "goal seek" function in the attached crappy 2 minute thrown-together spreadsheet, targeting 375 / 256. Approx a 200,000 fold improvement in tone spacing accuracy. Ain't that sweet?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click on Tools/Goal Seek, with cursor on I13 or L13 for target. Target value &lt; 0.04. Variable is $F9. If it doesn’t succeed, accept the best it got to update $F9. Int($F9) goes into the Den column, since the optimization creates a real.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://groups.io/g/picoballoon/topic/110236980#msg18933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">after hand experiments for 26Mhz tcxo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 10M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 12M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libreoffice goal seek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 15M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 17M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel similar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denom for 20M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Div 36 for 12M</t>
   </si>
   <si>
@@ -532,15 +559,6 @@
   </si>
   <si>
     <t xml:space="preserve">Div 42 for 15M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2M 456174 mul 33 div 6 (26Mhz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mult. Allow real for 2M?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremental shifts</t>
   </si>
 </sst>
 </file>
@@ -580,13 +598,6 @@
       <family val="0"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -596,6 +607,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -667,7 +685,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -696,7 +714,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -704,7 +722,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -720,7 +738,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,15 +754,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -756,7 +770,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,7 +960,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -954,8 +968,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
@@ -976,31 +990,19 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -1010,438 +1012,379 @@
         <f aca="false">D2*1.5</f>
         <v>2.197265625</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>28126020</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>28126180</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>24926020</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>24926180</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>21096020</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>21096180</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>28126180</v>
+        <v>144490500</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>28126177.8027344</v>
+        <v>144490497.802734</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>28126179.2675781</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>144490499.267578</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>28126180.7324219</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>14097020</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>14097180</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>18106020</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>18106180</v>
+        <v>144490500.732422</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>28126182.1972656</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>144490502.197266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>554667</v>
+        <v>505514</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="n">
-        <v>26000000</v>
+        <v>25000000</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>342139</v>
+        <v>264731.626748512</v>
       </c>
       <c r="E11" s="9" t="n">
-        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>554667</v>
+        <v>1048570</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>900037755.986925</v>
+        <v>581311729.945271</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>28126179.8745914</v>
+        <v>145327932.486318</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.07185704261065</v>
+        <v>837434.683583379</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
-        <f aca="false">D11+D17</f>
-        <v>342140</v>
-      </c>
-      <c r="E12" s="13"/>
+        <f aca="false">$D11 + D17</f>
+        <v>264731.626748512</v>
+      </c>
+      <c r="E12" s="13" t="n">
+        <f aca="false">E11-1</f>
+        <v>1048569</v>
+      </c>
       <c r="F12" s="10" t="n">
-        <f aca="false">B11*(C11+D12/E11)</f>
-        <v>900037802.861897</v>
+        <f aca="false">B11*(C11+D12/E12)</f>
+        <v>581311735.964646</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>28126181.3394343</v>
+        <v>145327933.991162</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46484287455678</v>
+        <v>1.50484374165535</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>-8.7544322013855E-007</v>
+        <v>0.0399999916553497</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>-0.87544322013855</v>
+        <v>39999.9916553497</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.07185616716743</v>
+        <v>837434.72358337</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.0311255626767625</v>
+        <v>275.239525924744</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>342141</v>
-      </c>
-      <c r="E13" s="13"/>
+        <v>264731.626748512</v>
+      </c>
+      <c r="E13" s="13" t="n">
+        <f aca="false">E11-2</f>
+        <v>1048568</v>
+      </c>
       <c r="F13" s="10" t="n">
-        <f aca="false">B11*(C11+D13/E11)</f>
-        <v>900037849.736869</v>
+        <f aca="false">B11*(C11+D13/E13)</f>
+        <v>581311741.984032</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>28126182.8042772</v>
+        <v>145327935.496008</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484287083149</v>
+        <v>1.5048466026783</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>-8.79168510437012E-007</v>
+        <v>0.040002852678299</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>-0.879168510437012</v>
+        <v>40002.852678299</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.07185528799891</v>
+        <v>837434.763586223</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>342142</v>
-      </c>
-      <c r="E14" s="13"/>
+        <v>264731.626748512</v>
+      </c>
+      <c r="E14" s="13" t="n">
+        <f aca="false">E11-3</f>
+        <v>1048567</v>
+      </c>
       <c r="F14" s="10" t="n">
-        <f aca="false">B11*(C11+D14/E11)</f>
-        <v>900037896.611841</v>
+        <f aca="false">B11*(C11+D14/E14)</f>
+        <v>581311748.00343</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>28126184.26912</v>
+        <v>145327937.000858</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484287083149</v>
+        <v>1.50484946370125</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>-8.79168510437012E-007</v>
+        <v>0.0400057137012482</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>-0.879168510437012</v>
+        <v>40005.7137012482</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.0718544088304</v>
+        <v>837434.803591937</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>900037760</v>
+        <v>577962000</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>28126180</v>
+        <v>144490500</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.6168369230769</v>
+        <v>23.11848</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.616836923076924</v>
+        <v>0.118480000000002</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>342139.085612308</v>
+        <v>124234.573600002</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="1" t="s">
-        <v>46</v>
+      <c r="G22" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -1449,46 +1392,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1514,7 +1457,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1561,30 +1504,30 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -1615,44 +1558,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>24926180</v>
+        <v>28126180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>24926177.8027344</v>
+        <v>28126177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>24926179.2675781</v>
+        <v>28126179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>24926180.7324219</v>
+        <v>28126180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -1670,83 +1613,80 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>24926182.1972656</v>
+        <v>28126182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>986074</v>
+        <v>554667</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,278 +1697,277 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>506026</v>
+        <v>342139</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>986074</v>
+        <v>554667</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>897342483.424165</v>
+        <v>900037755.986925</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>24926180.0951157</v>
+        <v>28126179.8745914</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.29238131642342</v>
+        <v>2.07185704261065</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>506028</v>
+        <v>342140</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>897342536.158544</v>
+        <v>900037802.861897</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>24926181.5599596</v>
+        <v>28126181.3394343</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46484386175871</v>
+        <v>1.46484287455678</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>1.11758708953857E-007</v>
+        <v>-8.7544322013855E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>0.111758708953857</v>
+        <v>-0.87544322013855</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.29238142818213</v>
+        <v>2.07185616716743</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.00448358721471331</v>
+        <v>0.0311255626767625</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>506030</v>
+        <v>342141</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>897342588.892923</v>
+        <v>900037849.736869</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>24926183.0248034</v>
+        <v>28126182.8042772</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484385803342</v>
+        <v>1.46484287083149</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>1.08033418655396E-007</v>
+        <v>-8.79168510437012E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>0.108033418655396</v>
+        <v>-0.879168510437012</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.29238153621554</v>
+        <v>2.07185528799891</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>506032</v>
+        <v>342142</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>897342641.627302</v>
+        <v>900037896.611841</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>24926184.4896473</v>
+        <v>28126184.26912</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484386175871</v>
+        <v>1.46484287083149</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>1.11758708953857E-007</v>
+        <v>-8.79168510437012E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>0.111758708953857</v>
+        <v>-0.879168510437012</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.29238164797425</v>
+        <v>2.0718544088304</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>897342480</v>
+        <v>900037760</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>24926180</v>
+        <v>28126180</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.5131723076923</v>
+        <v>34.6168369230769</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.513172307692308</v>
+        <v>0.616836923076924</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>506025.870135385</v>
+        <v>342139.085612308</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -2036,46 +1975,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2101,7 +2040,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2148,30 +2087,30 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -2202,44 +2141,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>21096180</v>
+        <v>24926180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>21096177.8027344</v>
+        <v>24926177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>21096179.2675781</v>
+        <v>24926179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>21096180.7324219</v>
+        <v>24926180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -2257,86 +2196,83 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>21096182.1972656</v>
+        <v>24926182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>845206</v>
+        <v>986074</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,278 +2283,277 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>66302</v>
+        <v>506026</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>845206</v>
+        <v>986074</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>886039564.319231</v>
+        <v>897342483.424165</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>21096180.1028388</v>
+        <v>24926180.0951157</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.30010445788503</v>
+        <v>2.29238131642342</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>66304</v>
+        <v>506028</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>886039625.842694</v>
+        <v>897342536.158544</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>21096181.5676832</v>
+        <v>24926181.5599596</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46484435722232</v>
+        <v>1.46484386175871</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>6.07222318649292E-007</v>
+        <v>1.11758708953857E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>0.607222318649292</v>
+        <v>0.111758708953857</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.30010506510735</v>
+        <v>2.29238142818213</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.0287835178466365</v>
+        <v>0.00448358721471331</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>66306</v>
+        <v>506030</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>886039687.366157</v>
+        <v>897342588.892923</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>21096183.0325275</v>
+        <v>24926183.0248034</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484435349703</v>
+        <v>1.46484385803342</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>6.0349702835083E-007</v>
+        <v>1.08033418655396E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>0.60349702835083</v>
+        <v>0.108033418655396</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.30010566860437</v>
+        <v>2.29238153621554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>66308</v>
+        <v>506032</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>886039748.88962</v>
+        <v>897342641.627302</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>21096184.4973719</v>
+        <v>24926184.4896473</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484435349703</v>
+        <v>1.46484386175871</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>6.0349702835083E-007</v>
+        <v>1.11758708953857E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>0.60349702835083</v>
+        <v>0.111758708953857</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.3001062721014</v>
+        <v>2.29238164797425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>886039560</v>
+        <v>897342480</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>21096180</v>
+        <v>24926180</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.0784446153846</v>
+        <v>34.5131723076923</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.0784446153846119</v>
+        <v>0.513172307692308</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>66301.8595907663</v>
+        <v>506025.870135385</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -2626,46 +2561,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2738,30 +2673,30 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -2792,38 +2727,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>18106020</v>
+        <v>21096180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>18106017.8027344</v>
+        <v>21096177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>18106019.2675781</v>
+        <v>21096179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>18106020.7324219</v>
+        <v>21096180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -2841,77 +2782,86 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>18106022.1972656</v>
+        <v>21096182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>69</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>1064960.885</v>
+        <v>845206</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,278 +2872,277 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>859065</v>
+        <v>66302</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>1048575</v>
+        <v>845206</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>905300994.206423</v>
+        <v>886039564.319231</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>18106019.8841285</v>
+        <v>21096180.1028388</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.08139408752322</v>
+        <v>2.30010445788503</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>859068</v>
+        <v>66304</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>905301068.593091</v>
+        <v>886039625.842694</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>18106021.3718618</v>
+        <v>21096181.5676832</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.48773334920406</v>
+        <v>1.46484435722232</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>0.0228895992040634</v>
+        <v>6.07222318649292E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>22889.5992040634</v>
+        <v>0.607222318649292</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.10428368672729</v>
+        <v>2.30010506510735</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>1264.19817661519</v>
+        <v>0.0287835178466365</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>859071</v>
+        <v>66306</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>905301142.979758</v>
+        <v>886039687.366157</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>18106022.8595952</v>
+        <v>21096183.0325275</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.48773335292935</v>
+        <v>1.46484435349703</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>6.0349702835083E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>22889.6029293537</v>
+        <v>0.60349702835083</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.12717328965664</v>
+        <v>2.30010566860437</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>859074</v>
+        <v>66308</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>905301217.366426</v>
+        <v>886039748.88962</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>18106024.3473285</v>
+        <v>21096184.4973719</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.48773335292935</v>
+        <v>1.46484435349703</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>6.0349702835083E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>22889.6029293537</v>
+        <v>0.60349702835083</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.15006289258599</v>
+        <v>2.3001062721014</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>905301000</v>
+        <v>886039560</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>18106020</v>
+        <v>21096180</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.8192692307692</v>
+        <v>34.0784446153846</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.81926923076923</v>
+        <v>0.0784446153846119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>859065.233653845</v>
+        <v>66301.8595907663</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -3201,46 +3150,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3313,30 +3262,30 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -3367,38 +3316,38 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>14097180</v>
+        <v>18106020</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>14097177.8027344</v>
+        <v>18106017.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>14097179.2675781</v>
+        <v>18106019.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>14097180.7324219</v>
+        <v>18106020.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -3416,80 +3365,77 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>14097182.1972656</v>
+        <v>18106022.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>277333</v>
+        <v>1064960.885</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,278 +3446,277 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>194341</v>
+        <v>859065</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>277333</v>
+        <v>1048575</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>902219490.648426</v>
+        <v>905300994.206423</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>14097179.5413817</v>
+        <v>18106019.8841285</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>1.73864728398621</v>
+        <v>2.08139408752322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>194342</v>
+        <v>859068</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>902219584.398539</v>
+        <v>905301068.593091</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>14097181.0062272</v>
+        <v>18106021.3718618</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46484551392496</v>
+        <v>1.48773334920406</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>1.76392495632172E-006</v>
+        <v>0.0228895992040634</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>1.76392495632172</v>
+        <v>22889.5992040634</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>1.73864904791117</v>
+        <v>2.10428368672729</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.125126077017989</v>
+        <v>1264.19817661519</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>194343</v>
+        <v>859071</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>902219678.148652</v>
+        <v>905301142.979758</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>14097182.4710727</v>
+        <v>18106022.8595952</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484551019967</v>
+        <v>1.48773335292935</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>1.76019966602325E-006</v>
+        <v>0.0228896029293537</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>1.76019966602325</v>
+        <v>22889.6029293537</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>1.73865080811083</v>
+        <v>2.12717328965664</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>194344</v>
+        <v>859074</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>902219771.898764</v>
+        <v>905301217.366426</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>14097183.9359182</v>
+        <v>18106024.3473285</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484551019967</v>
+        <v>1.48773335292935</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>1.76019966602325E-006</v>
+        <v>0.0228896029293537</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>1.76019966602325</v>
+        <v>22889.6029293537</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>1.7386525683105</v>
+        <v>2.15006289258599</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>902219520</v>
+        <v>905301000</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>14097180</v>
+        <v>18106020</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.7007507692308</v>
+        <v>34.8192692307692</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.700750769230773</v>
+        <v>0.81926923076923</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>194341.313083078</v>
+        <v>859065.233653845</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -3779,46 +3724,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3860,7 +3805,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3891,30 +3836,30 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">375/256</f>
@@ -3945,44 +3890,38 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>144885180</v>
+        <v>14097180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>144885177.802734</v>
+        <v>14097177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>144885179.267578</v>
+        <v>14097179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>144885180.732422</v>
+        <v>14097180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -4000,83 +3939,80 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>144885182.197266</v>
+        <v>14097182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>1973529.60362751</v>
+        <v>277333</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G10" s="8"/>
-      <c r="H10" s="17" t="s">
-        <v>75</v>
+      <c r="H10" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4084,284 +4020,280 @@
         <v>26000000</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>100</v>
+        <v>194341</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>1048575</v>
+        <v>277333</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>1040002479.55559</v>
+        <v>902219490.648426</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>104000247.955559</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>54</v>
+        <v>14097179.5413817</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>-40884929.8471756</v>
+        <v>1.73864728398621</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
-        <f aca="false">$D11 + D17</f>
-        <v>101</v>
+        <f aca="false">D11+D17</f>
+        <v>194342</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>1040002504.35114</v>
+        <v>902219584.398539</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>104000250.435114</v>
+        <v>14097181.0062272</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>2.47955559194088</v>
+        <v>1.46484551392496</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>1.01471184194088</v>
+        <v>1.76392495632172E-006</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>1014711.84194088</v>
+        <v>1.76392495632172</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>-40884928.8324638</v>
+        <v>1.73864904791117</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>9756.82113932945</v>
+        <v>0.125126077017989</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>102</v>
+        <v>194343</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>1040002529.1467</v>
+        <v>902219678.148652</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>104000252.91467</v>
+        <v>14097182.4710727</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>2.47955557703972</v>
+        <v>1.46484551019967</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>1.01471182703972</v>
+        <v>1.76019966602325E-006</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>1014711.82703972</v>
+        <v>1.76019966602325</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>-40884927.817752</v>
+        <v>1.73865080811083</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>103</v>
+        <v>194344</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>1040002553.94226</v>
+        <v>902219771.898764</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>104000255.394226</v>
+        <v>14097183.9359182</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>2.47955560684204</v>
+        <v>1.46484551019967</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>1.01471185684204</v>
+        <v>1.76019966602325E-006</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>1014711.85684204</v>
+        <v>1.76019966602325</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>-40884926.8030401</v>
+        <v>1.7386525683105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>1448851800</v>
+        <v>902219520</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>144885180</v>
+        <v>14097180</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>55.7250692307692</v>
+        <v>34.7007507692308</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
       <c r="E18" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>15.7250692307692</v>
+        <v>0.700750769230773</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="18" t="n">
+      <c r="C19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>16488914.4686538</v>
+        <v>194341.313083078</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L23" s="5" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="A26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="A27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="L27" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="B29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="L29" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>554667</v>
@@ -4369,46 +4301,46 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I33" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="C37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
some tweaks for the solar functions
</commit_message>
<xml_diff>
--- a/tracker/WSPRDenom-modified.xlsx
+++ b/tracker/WSPRDenom-modified.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10M 390Mhz denom shift2" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="10M 500 Mhz denom shift2" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="2M hans denom shift" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="10M" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="12M" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="15M" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="17M" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="20M" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="10M 390Mhz denom shift3" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="10M 500 Mhz denom shift2" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="2M hans denom shift" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="10M" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="12M" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="15M" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="17M" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="20M" sheetId="9" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_adj" vbProcedure="false">'10M 390Mhz denom shift2'!F9</definedName>
@@ -40,7 +41,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="solver_tim" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_typ" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_vrt" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="solver_adj" vbProcedure="false">'10M 500 Mhz denom shift2'!F9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="solver_adj" vbProcedure="false">'10M 390Mhz denom shift3'!F9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_alg" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_asr" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_bbd" vbProcedure="false">0</definedName>
@@ -54,7 +55,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="solver_mtpb" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_neg" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_num" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="solver_opt" vbProcedure="false">'10M 500 Mhz denom shift2'!L11</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="solver_opt" vbProcedure="false">'10M 390Mhz denom shift3'!L11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_smax" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_smin" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_soc" vbProcedure="false">0</definedName>
@@ -62,31 +63,53 @@
     <definedName function="false" hidden="false" localSheetId="1" name="solver_tim" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_typ" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="solver_vrt" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_adj" vbProcedure="false">'2M hans denom shift'!F9</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_adj" vbProcedure="false">'10M 500 Mhz denom shift2'!F9</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_alg" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_asr" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_bbd" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_bbd" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_ccoeff" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_cog" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_crpb" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_eng" vbProcedure="false">1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_eps" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_eng" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_eps" vbProcedure="false">3</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_int" vbProcedure="false">1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_lhs1" vbProcedure="false">'2M hans denom shift'!D11</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_lo_eng" vbProcedure="false">"com.sun.star.comp.Calc.SwarmSolver"</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_lo_eng" vbProcedure="false">"com.sun.star.comp.Calc.LpsolveSolver"</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_mtpb" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_neg" vbProcedure="false">1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_num" vbProcedure="false">1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_opt" vbProcedure="false">'2M hans denom shift'!L11</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_rel1" vbProcedure="false">1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_rhs1" vbProcedure="false">'2M hans denom shift'!E11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_num" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_opt" vbProcedure="false">'10M 500 Mhz denom shift2'!L11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_smax" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_smin" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_soc" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_stol" vbProcedure="false">0</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="solver_tim" vbProcedure="false">60000</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="solver_tim" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_typ" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="solver_vrt" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_adj" vbProcedure="false">'2M hans denom shift'!F9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_alg" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_asr" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_bbd" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_ccoeff" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_cog" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_crpb" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_eng" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_eps" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_int" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_lhs1" vbProcedure="false">'2M hans denom shift'!D11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_lo_eng" vbProcedure="false">"com.sun.star.comp.Calc.SwarmSolver"</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_mtpb" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_neg" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_num" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_opt" vbProcedure="false">'2M hans denom shift'!L11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_rel1" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_rhs1" vbProcedure="false">'2M hans denom shift'!E11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_smax" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_smin" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_soc" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_stol" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_tim" vbProcedure="false">60000</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_typ" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="solver_vrt" vbProcedure="false">0</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -98,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="93">
   <si>
     <t xml:space="preserve">adjust for band/channel</t>
   </si>
@@ -251,6 +274,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denominator</t>
   </si>
   <si>
     <t xml:space="preserve">Mult. Allow real for 2M?</t>
@@ -779,7 +814,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -870,6 +905,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1057,7 +1096,7 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1582,8 +1621,8 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1673,33 +1712,33 @@
         <v>6</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
-        <v>7</v>
+      <c r="H8" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>928898</v>
+        <v>550999</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
+      <c r="C10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -1728,22 +1767,22 @@
         <v>26000000</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>438412</v>
+        <v>79821</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">INT(F9)</f>
-        <v>928898</v>
+        <v>550999</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>506271220.306212</v>
+        <v>393766515.00275</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>28126178.9059007</v>
+        <v>28126179.6430535</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>19</v>
@@ -1751,117 +1790,117 @@
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>1.103166308254</v>
+        <v>1.84031916409731</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">$D11 + D17</f>
-        <v>438412</v>
+        <v>79821</v>
       </c>
       <c r="E12" s="13" t="n">
         <f aca="false">E11-E16</f>
-        <v>928896</v>
+        <v>550996</v>
       </c>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E12)</f>
-        <v>506271246.727298</v>
+        <v>393766535.51024</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>28126180.3737388</v>
+        <v>28126181.1078743</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46783808246255</v>
+        <v>1.46482072398067</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>0.00299433246254921</v>
+        <v>-2.30260193347931E-005</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>2994.33246254921</v>
+        <v>-23.0260193347931</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>1.10616064071655</v>
+        <v>1.84029613807797</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>106.460686192036</v>
+        <v>0.81866852974031</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>438412</v>
+        <v>79821</v>
       </c>
       <c r="E13" s="13" t="n">
         <f aca="false">E12-E16</f>
-        <v>928894</v>
+        <v>550993</v>
       </c>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E13)</f>
-        <v>506271273.148497</v>
+        <v>393766556.017953</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>28126181.8415832</v>
+        <v>28126182.5727109</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.4678444005549</v>
+        <v>1.46483666822314</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>0.0030006505548954</v>
+        <v>-7.0817768573761E-006</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>3000.6505548954</v>
+        <v>-7.0817768573761</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>1.10916129127145</v>
+        <v>1.84028905630112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>438412</v>
+        <v>79821</v>
       </c>
       <c r="E14" s="13" t="n">
         <f aca="false">E13-E16</f>
-        <v>928892</v>
+        <v>550990</v>
       </c>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E14)</f>
-        <v>506271299.56981</v>
+        <v>393766576.52589</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>28126183.3094339</v>
+        <v>28126184.0375636</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46785072609782</v>
+        <v>1.46485262364149</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>0.00300697609782219</v>
+        <v>8.87364149093628E-006</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>3006.97609782219</v>
+        <v>8.87364149093628</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>1.11216826736927</v>
+        <v>1.84029792994261</v>
       </c>
       <c r="L14" s="16" t="n">
         <f aca="false">ABS(1000000*J14/G14)</f>
-        <v>106.910207643197</v>
+        <v>0.315493970994615</v>
       </c>
       <c r="M14" s="17" t="s">
         <v>20</v>
@@ -1886,11 +1925,11 @@
         <v>23</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>506271240</v>
+        <v>393766520</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
@@ -1914,7 +1953,7 @@
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>19.4719707692308</v>
+        <v>15.1448661538462</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,7 +1962,7 @@
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.471970769230769</v>
+        <v>0.144866153846154</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1977,7 @@
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>438412.703596923</v>
+        <v>79821.105903077</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>30</v>
@@ -2107,24 +2146,24 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2163,11 +2202,11 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>144490500</v>
+        <v>28126180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>144490497.802734</v>
+        <v>28126177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,19 +2215,19 @@
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>144490499.267578</v>
+        <v>28126179.2675781</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>144490500.732422</v>
+        <v>28126180.7324219</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>144490502.197266</v>
+        <v>28126182.1972656</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,17 +2237,19 @@
         <v>6</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>505966.054320736</v>
+        <v>928898</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,7 +2257,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -2248,25 +2289,25 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="n">
-        <v>25000000</v>
+        <v>26000000</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>60000</v>
+        <v>438412</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">INT(F9)</f>
-        <v>505966</v>
+        <v>928898</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>577964626.081595</v>
+        <v>506271220.306212</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>144491156.520399</v>
+        <v>28126178.9059007</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>19</v>
@@ -2274,123 +2315,117 @@
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>658.717664241791</v>
+        <v>1.103166308254</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">$D11 + D17</f>
-        <v>60000</v>
+        <v>438412</v>
       </c>
       <c r="E12" s="13" t="n">
-        <f aca="false">E11-1</f>
-        <v>505965</v>
+        <f aca="false">E11-E16</f>
+        <v>928896</v>
       </c>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E12)</f>
-        <v>577964631.940945</v>
+        <v>506271246.727298</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>144491157.985236</v>
+        <v>28126180.3737388</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46483752131462</v>
+        <v>1.46783808246255</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>-6.22868537902832E-006</v>
+        <v>0.00299433246254921</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>-6.22868537902832</v>
+        <v>2994.33246254921</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>658.717658013105</v>
+        <v>1.10616064071655</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.0431077269078621</v>
+        <v>106.460686192036</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>60000</v>
+        <v>438412</v>
       </c>
       <c r="E13" s="13" t="n">
-        <f aca="false">E11-2</f>
-        <v>505964</v>
+        <f aca="false">E12-E16</f>
+        <v>928894</v>
       </c>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E13)</f>
-        <v>577964637.800318</v>
+        <v>506271273.148497</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>144491159.450079</v>
+        <v>28126181.8415832</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484330296516</v>
+        <v>1.4678444005549</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>-4.4703483581543E-007</v>
+        <v>0.0030006505548954</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>-0.44703483581543</v>
+        <v>3000.6505548954</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>658.717657566071</v>
+        <v>1.10916129127145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>60000</v>
+        <v>438412</v>
       </c>
       <c r="E14" s="13" t="n">
-        <f aca="false">E11-3</f>
-        <v>505963</v>
+        <f aca="false">E13-E16</f>
+        <v>928892</v>
       </c>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E14)</f>
-        <v>577964643.659714</v>
+        <v>506271299.56981</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>144491160.914929</v>
+        <v>28126183.3094339</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484911441803</v>
+        <v>1.46785072609782</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>5.36441802978516E-006</v>
+        <v>0.00300697609782219</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>5.36441802978516</v>
+        <v>3006.97609782219</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>658.717662930489</v>
+        <v>1.11216826736927</v>
       </c>
       <c r="L14" s="16" t="n">
         <f aca="false">ABS(1000000*J14/G14)</f>
-        <v>0.0371262712252934</v>
+        <v>106.910207643197</v>
       </c>
       <c r="M14" s="17" t="s">
         <v>20</v>
@@ -2399,10 +2434,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
@@ -2412,16 +2447,18 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>577962000</v>
+        <v>506271240</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>144490500</v>
+        <v>28126180</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>24</v>
@@ -2441,7 +2478,7 @@
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>23.11848</v>
+        <v>19.4719707692308</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2487,7 @@
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.118480000000002</v>
+        <v>0.471970769230769</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2502,7 @@
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>59946.8516800009</v>
+        <v>438412.703596923</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>30</v>
@@ -2474,9 +2511,6 @@
       <c r="K19" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G22" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="L22" s="5" t="s">
         <v>31</v>
       </c>
@@ -2599,11 +2633,10 @@
       <c r="I37" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="M14:N15"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="I19:K19"/>
@@ -2638,6 +2671,537 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>144490500</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>144490497.802734</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>144490499.267578</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>144490500.732422</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>144490502.197266</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>505966.054320736</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>25000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>60000</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">INT(F9)</f>
+        <v>505966</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>577964626.081595</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>144491156.520399</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>658.717664241791</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">$D11 + D17</f>
+        <v>60000</v>
+      </c>
+      <c r="E12" s="13" t="n">
+        <f aca="false">E11-1</f>
+        <v>505965</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E12)</f>
+        <v>577964631.940945</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>144491157.985236</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.46483752131462</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>-6.22868537902832E-006</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>-6.22868537902832</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>658.717658013105</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>0.0431077269078621</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>60000</v>
+      </c>
+      <c r="E13" s="13" t="n">
+        <f aca="false">E11-2</f>
+        <v>505964</v>
+      </c>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E13)</f>
+        <v>577964637.800318</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>144491159.450079</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.46484330296516</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>-4.4703483581543E-007</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>-0.44703483581543</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>658.717657566071</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>60000</v>
+      </c>
+      <c r="E14" s="13" t="n">
+        <f aca="false">E11-3</f>
+        <v>505963</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E14)</f>
+        <v>577964643.659714</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>144491160.914929</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.46484911441803</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>5.36441802978516E-006</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>5.36441802978516</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>658.717662930489</v>
+      </c>
+      <c r="L14" s="16" t="n">
+        <f aca="false">ABS(1000000*J14/G14)</f>
+        <v>0.0371262712252934</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="17"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>577962000</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>144490500</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>23.11848</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.118480000000002</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>59946.8516800009</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="M14:N15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
@@ -2670,22 +3234,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,35 +3297,35 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
         <v>28126179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
         <v>28126180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -2782,23 +3346,23 @@
         <v>28126182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
@@ -2806,12 +3370,12 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
@@ -2827,7 +3391,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -2840,7 +3404,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
@@ -2985,7 +3549,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
@@ -3048,12 +3612,12 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>31</v>
@@ -3070,7 +3634,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>33</v>
@@ -3080,7 +3644,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>34</v>
@@ -3207,592 +3771,6 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:P37"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <f aca="false">375/256</f>
-        <v>1.46484375</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">D2*1.5</f>
-        <v>2.197265625</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>28126020</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>28126180</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>24926020</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>24926180</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>21096020</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>21096180</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="n">
-        <v>24926180</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <f aca="false">B3-E2</f>
-        <v>24926177.8027344</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <f aca="false">C3+$D$2</f>
-        <v>24926179.2675781</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <f aca="false">C4+$D$2</f>
-        <v>24926180.7324219</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>14097020</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>14097180</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>18106020</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>18106180</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4" t="n">
-        <f aca="false">C5+$D$2</f>
-        <v>24926182.1972656</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7" t="n">
-        <v>986074</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="3" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="n">
-        <v>26000000</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>506026</v>
-      </c>
-      <c r="E11" s="9" t="n">
-        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>986074</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <f aca="false">B11*(C11+D11/E11)</f>
-        <v>897342483.424165</v>
-      </c>
-      <c r="G11" s="11" t="n">
-        <f aca="false">F11/H9</f>
-        <v>24926180.0951157</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="12" t="n">
-        <f aca="false">G11-C3</f>
-        <v>2.29238131642342</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="1" t="n">
-        <f aca="false">D11+D17</f>
-        <v>506028</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="10" t="n">
-        <f aca="false">B11*(C11+D12/E11)</f>
-        <v>897342536.158544</v>
-      </c>
-      <c r="G12" s="11" t="n">
-        <f aca="false">F12/H9</f>
-        <v>24926181.5599596</v>
-      </c>
-      <c r="H12" s="14" t="n">
-        <f aca="false">G12-G11</f>
-        <v>1.46484386175871</v>
-      </c>
-      <c r="I12" s="15" t="n">
-        <f aca="false">H12-$D$2</f>
-        <v>1.11758708953857E-007</v>
-      </c>
-      <c r="J12" s="10" t="n">
-        <f aca="false">I12*1000000</f>
-        <v>0.111758708953857</v>
-      </c>
-      <c r="K12" s="12" t="n">
-        <f aca="false">G12-C4</f>
-        <v>2.29238142818213</v>
-      </c>
-      <c r="L12" s="16" t="n">
-        <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.00448358721471331</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="1" t="n">
-        <f aca="false">D12+D17</f>
-        <v>506030</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="10" t="n">
-        <f aca="false">B11*(C11+D13/E11)</f>
-        <v>897342588.892923</v>
-      </c>
-      <c r="G13" s="11" t="n">
-        <f aca="false">F13/H9</f>
-        <v>24926183.0248034</v>
-      </c>
-      <c r="H13" s="14" t="n">
-        <f aca="false">G13-G12</f>
-        <v>1.46484385803342</v>
-      </c>
-      <c r="I13" s="14" t="n">
-        <f aca="false">H13-$D$2</f>
-        <v>1.08033418655396E-007</v>
-      </c>
-      <c r="J13" s="10" t="n">
-        <f aca="false">I13*1000000</f>
-        <v>0.108033418655396</v>
-      </c>
-      <c r="K13" s="12" t="n">
-        <f aca="false">G13-C5</f>
-        <v>2.29238153621554</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="1" t="n">
-        <f aca="false">D13+D17</f>
-        <v>506032</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="10" t="n">
-        <f aca="false">B11*(C11+D14/E11)</f>
-        <v>897342641.627302</v>
-      </c>
-      <c r="G14" s="11" t="n">
-        <f aca="false">F14/H9</f>
-        <v>24926184.4896473</v>
-      </c>
-      <c r="H14" s="14" t="n">
-        <f aca="false">G14-G13</f>
-        <v>1.46484386175871</v>
-      </c>
-      <c r="I14" s="14" t="n">
-        <f aca="false">H14-$D$2</f>
-        <v>1.11758708953857E-007</v>
-      </c>
-      <c r="J14" s="10" t="n">
-        <f aca="false">I14*1000000</f>
-        <v>0.111758708953857</v>
-      </c>
-      <c r="K14" s="12" t="n">
-        <f aca="false">G14-C6</f>
-        <v>2.29238164797425</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="1" t="n">
-        <f aca="false">B3*H9</f>
-        <v>897342480</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <f aca="false">B3</f>
-        <v>24926180</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <f aca="false">F16/B11</f>
-        <v>34.5131723076923</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <f aca="false">F17-C11</f>
-        <v>0.513172307692308</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <f aca="false">F18*E11</f>
-        <v>506025.870135385</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="L27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="L29" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="I31" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="1" t="n">
-        <v>554667</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="I35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="L29:P29"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C37:I37"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
-    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3839,22 +3817,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,44 +3871,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>21096180</v>
+        <v>24926180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>21096177.8027344</v>
+        <v>24926177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>21096179.2675781</v>
+        <v>24926179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>21096180.7324219</v>
+        <v>24926180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -3948,29 +3926,26 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>21096182.1972656</v>
+        <v>24926182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
@@ -3978,23 +3953,23 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>845206</v>
+        <v>986074</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4002,7 +3977,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -4015,7 +3990,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
@@ -4038,121 +4013,121 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>66302</v>
+        <v>506026</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>845206</v>
+        <v>986074</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>886039564.319231</v>
+        <v>897342483.424165</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>21096180.1028388</v>
+        <v>24926180.0951157</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.30010445788503</v>
+        <v>2.29238131642342</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>66304</v>
+        <v>506028</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>886039625.842694</v>
+        <v>897342536.158544</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>21096181.5676832</v>
+        <v>24926181.5599596</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.46484435722232</v>
+        <v>1.46484386175871</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>6.07222318649292E-007</v>
+        <v>1.11758708953857E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>0.607222318649292</v>
+        <v>0.111758708953857</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.30010506510735</v>
+        <v>2.29238142818213</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>0.0287835178466365</v>
+        <v>0.00448358721471331</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>66306</v>
+        <v>506030</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>886039687.366157</v>
+        <v>897342588.892923</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>21096183.0325275</v>
+        <v>24926183.0248034</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.46484435349703</v>
+        <v>1.46484385803342</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>6.0349702835083E-007</v>
+        <v>1.08033418655396E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>0.60349702835083</v>
+        <v>0.108033418655396</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.30010566860437</v>
+        <v>2.29238153621554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>66308</v>
+        <v>506032</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>886039748.88962</v>
+        <v>897342641.627302</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>21096184.4973719</v>
+        <v>24926184.4896473</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.46484435349703</v>
+        <v>1.46484386175871</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>6.0349702835083E-007</v>
+        <v>1.11758708953857E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>0.60349702835083</v>
+        <v>0.111758708953857</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.3001062721014</v>
+        <v>2.29238164797425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4160,16 +4135,16 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>886039560</v>
+        <v>897342480</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>21096180</v>
+        <v>24926180</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>24</v>
@@ -4189,7 +4164,7 @@
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.0784446153846</v>
+        <v>34.5131723076923</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4198,7 +4173,7 @@
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.0784446153846119</v>
+        <v>0.513172307692308</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4213,7 +4188,7 @@
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>66301.8595907663</v>
+        <v>506025.870135385</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>30</v>
@@ -4223,12 +4198,12 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>31</v>
@@ -4245,7 +4220,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>33</v>
@@ -4255,7 +4230,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>34</v>
@@ -4428,22 +4403,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,38 +4457,44 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="n">
-        <v>18106020</v>
+        <v>21096180</v>
       </c>
       <c r="C3" s="4" t="n">
         <f aca="false">B3-E2</f>
-        <v>18106017.8027344</v>
+        <v>21096177.8027344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C4" s="4" t="n">
         <f aca="false">C3+$D$2</f>
-        <v>18106019.2675781</v>
+        <v>21096179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="C5" s="4" t="n">
         <f aca="false">C4+$D$2</f>
-        <v>18106020.7324219</v>
+        <v>21096180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -4531,23 +4512,29 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="4" t="n">
         <f aca="false">C5+$D$2</f>
-        <v>18106022.1972656</v>
+        <v>21096182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
@@ -4555,20 +4542,23 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
-        <v>1064960.885</v>
+        <v>845206</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4576,7 +4566,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -4589,7 +4579,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
@@ -4612,121 +4602,121 @@
         <v>34</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>859065</v>
+        <v>66302</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
-        <v>1048575</v>
+        <v>845206</v>
       </c>
       <c r="F11" s="10" t="n">
         <f aca="false">B11*(C11+D11/E11)</f>
-        <v>905300994.206423</v>
+        <v>886039564.319231</v>
       </c>
       <c r="G11" s="11" t="n">
         <f aca="false">F11/H9</f>
-        <v>18106019.8841285</v>
+        <v>21096180.1028388</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="12" t="n">
         <f aca="false">G11-C3</f>
-        <v>2.08139408752322</v>
+        <v>2.30010445788503</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="1" t="n">
         <f aca="false">D11+D17</f>
-        <v>859068</v>
+        <v>66304</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="10" t="n">
         <f aca="false">B11*(C11+D12/E11)</f>
-        <v>905301068.593091</v>
+        <v>886039625.842694</v>
       </c>
       <c r="G12" s="11" t="n">
         <f aca="false">F12/H9</f>
-        <v>18106021.3718618</v>
+        <v>21096181.5676832</v>
       </c>
       <c r="H12" s="14" t="n">
         <f aca="false">G12-G11</f>
-        <v>1.48773334920406</v>
+        <v>1.46484435722232</v>
       </c>
       <c r="I12" s="15" t="n">
         <f aca="false">H12-$D$2</f>
-        <v>0.0228895992040634</v>
+        <v>6.07222318649292E-007</v>
       </c>
       <c r="J12" s="10" t="n">
         <f aca="false">I12*1000000</f>
-        <v>22889.5992040634</v>
+        <v>0.607222318649292</v>
       </c>
       <c r="K12" s="12" t="n">
         <f aca="false">G12-C4</f>
-        <v>2.10428368672729</v>
+        <v>2.30010506510735</v>
       </c>
       <c r="L12" s="16" t="n">
         <f aca="false">ABS(1000000*J12/G12)</f>
-        <v>1264.19817661519</v>
+        <v>0.0287835178466365</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="n">
         <f aca="false">D12+D17</f>
-        <v>859071</v>
+        <v>66306</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="10" t="n">
         <f aca="false">B11*(C11+D13/E11)</f>
-        <v>905301142.979758</v>
+        <v>886039687.366157</v>
       </c>
       <c r="G13" s="11" t="n">
         <f aca="false">F13/H9</f>
-        <v>18106022.8595952</v>
+        <v>21096183.0325275</v>
       </c>
       <c r="H13" s="14" t="n">
         <f aca="false">G13-G12</f>
-        <v>1.48773335292935</v>
+        <v>1.46484435349703</v>
       </c>
       <c r="I13" s="14" t="n">
         <f aca="false">H13-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>6.0349702835083E-007</v>
       </c>
       <c r="J13" s="10" t="n">
         <f aca="false">I13*1000000</f>
-        <v>22889.6029293537</v>
+        <v>0.60349702835083</v>
       </c>
       <c r="K13" s="12" t="n">
         <f aca="false">G13-C5</f>
-        <v>2.12717328965664</v>
+        <v>2.30010566860437</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="1" t="n">
         <f aca="false">D13+D17</f>
-        <v>859074</v>
+        <v>66308</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10" t="n">
         <f aca="false">B11*(C11+D14/E11)</f>
-        <v>905301217.366426</v>
+        <v>886039748.88962</v>
       </c>
       <c r="G14" s="11" t="n">
         <f aca="false">F14/H9</f>
-        <v>18106024.3473285</v>
+        <v>21096184.4973719</v>
       </c>
       <c r="H14" s="14" t="n">
         <f aca="false">G14-G13</f>
-        <v>1.48773335292935</v>
+        <v>1.46484435349703</v>
       </c>
       <c r="I14" s="14" t="n">
         <f aca="false">H14-$D$2</f>
-        <v>0.0228896029293537</v>
+        <v>6.0349702835083E-007</v>
       </c>
       <c r="J14" s="10" t="n">
         <f aca="false">I14*1000000</f>
-        <v>22889.6029293537</v>
+        <v>0.60349702835083</v>
       </c>
       <c r="K14" s="12" t="n">
         <f aca="false">G14-C6</f>
-        <v>2.15006289258599</v>
+        <v>2.3001062721014</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,16 +4724,16 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
         <f aca="false">B3*H9</f>
-        <v>905301000</v>
+        <v>886039560</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">B3</f>
-        <v>18106020</v>
+        <v>21096180</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>24</v>
@@ -4756,14 +4746,14 @@
         <v>25</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">F16/B11</f>
-        <v>34.8192692307692</v>
+        <v>34.0784446153846</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4772,7 +4762,7 @@
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">F17-C11</f>
-        <v>0.81926923076923</v>
+        <v>0.0784446153846119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4787,7 +4777,7 @@
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">F18*E11</f>
-        <v>859065.233653845</v>
+        <v>66301.8595907663</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>30</v>
@@ -4797,12 +4787,12 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>31</v>
@@ -4819,7 +4809,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>33</v>
@@ -4829,7 +4819,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>34</v>
@@ -4971,6 +4961,580 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="false">375/256</f>
+        <v>1.46484375</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2*1.5</f>
+        <v>2.197265625</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>28126020</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>28126180</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>24926020</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>24926180</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>21096020</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>21096180</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <f aca="false">B3-E2</f>
+        <v>18106017.8027344</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="n">
+        <f aca="false">C3+$D$2</f>
+        <v>18106019.2675781</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="4" t="n">
+        <f aca="false">C4+$D$2</f>
+        <v>18106020.7324219</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>14097020</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>14097180</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>18106020</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>18106180</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4" t="n">
+        <f aca="false">C5+$D$2</f>
+        <v>18106022.1972656</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="n">
+        <v>1064960.885</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>859065</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">IF(F9&lt;1048575, INT(F9), 1048575)</f>
+        <v>1048575</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <f aca="false">B11*(C11+D11/E11)</f>
+        <v>905300994.206423</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">F11/H9</f>
+        <v>18106019.8841285</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="12" t="n">
+        <f aca="false">G11-C3</f>
+        <v>2.08139408752322</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1" t="n">
+        <f aca="false">D11+D17</f>
+        <v>859068</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="10" t="n">
+        <f aca="false">B11*(C11+D12/E11)</f>
+        <v>905301068.593091</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <f aca="false">F12/H9</f>
+        <v>18106021.3718618</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <f aca="false">G12-G11</f>
+        <v>1.48773334920406</v>
+      </c>
+      <c r="I12" s="15" t="n">
+        <f aca="false">H12-$D$2</f>
+        <v>0.0228895992040634</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <f aca="false">I12*1000000</f>
+        <v>22889.5992040634</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <f aca="false">G12-C4</f>
+        <v>2.10428368672729</v>
+      </c>
+      <c r="L12" s="16" t="n">
+        <f aca="false">ABS(1000000*J12/G12)</f>
+        <v>1264.19817661519</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1" t="n">
+        <f aca="false">D12+D17</f>
+        <v>859071</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="10" t="n">
+        <f aca="false">B11*(C11+D13/E11)</f>
+        <v>905301142.979758</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <f aca="false">F13/H9</f>
+        <v>18106022.8595952</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <f aca="false">G13-G12</f>
+        <v>1.48773335292935</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <f aca="false">H13-$D$2</f>
+        <v>0.0228896029293537</v>
+      </c>
+      <c r="J13" s="10" t="n">
+        <f aca="false">I13*1000000</f>
+        <v>22889.6029293537</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <f aca="false">G13-C5</f>
+        <v>2.12717328965664</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13+D17</f>
+        <v>859074</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="10" t="n">
+        <f aca="false">B11*(C11+D14/E11)</f>
+        <v>905301217.366426</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <f aca="false">F14/H9</f>
+        <v>18106024.3473285</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <f aca="false">G14-G13</f>
+        <v>1.48773335292935</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <f aca="false">H14-$D$2</f>
+        <v>0.0228896029293537</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <f aca="false">I14*1000000</f>
+        <v>22889.6029293537</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <f aca="false">G14-C6</f>
+        <v>2.15006289258599</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1" t="n">
+        <f aca="false">B3*H9</f>
+        <v>905301000</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">B3</f>
+        <v>18106020</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16/B11</f>
+        <v>34.8192692307692</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17-C11</f>
+        <v>0.81926923076923</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18*E11</f>
+        <v>859065.233653845</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="L27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="L29" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="I31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>554667</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="I35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="L29:P29"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C37:I37"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -5002,22 +5566,22 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,16 +5633,16 @@
         <v>14097179.2675781</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5087,7 +5651,7 @@
         <v>14097180.7324219</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>14097020</v>
@@ -5108,23 +5672,23 @@
         <v>14097182.1972656</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
@@ -5132,12 +5696,12 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="7" t="n">
@@ -5153,7 +5717,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -5166,7 +5730,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
@@ -5311,7 +5875,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1" t="n">
@@ -5374,12 +5938,12 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>31</v>
@@ -5396,7 +5960,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>33</v>
@@ -5406,7 +5970,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
I only had one function that returned uint64_t. I think occasionly it would just return the upper 32 bits?
   freq_xxx = calcSymbolFreq_xxx(xmit_freq, symbol);
I just changed it to pass a pointer as the first arg instead. seems more reliable and not-unique-behavior
Showed up when I was doing larger PLL_CALC_SHIFT values
</commit_message>
<xml_diff>
--- a/tracker/WSPRDenom-modified.xlsx
+++ b/tracker/WSPRDenom-modified.xlsx
@@ -704,7 +704,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.0000"/>
     <numFmt numFmtId="171" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -734,6 +734,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -814,7 +822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -909,6 +917,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1622,7 +1634,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2019,11 +2031,11 @@
       <c r="C26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="L27" s="5" t="s">
         <v>37</v>
       </c>
@@ -2108,7 +2120,7 @@
       <c r="I37" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="M14:N15"/>
@@ -2118,6 +2130,7 @@
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="L23:N23"/>
     <mergeCell ref="L24:N24"/>
+    <mergeCell ref="A27:C27"/>
     <mergeCell ref="L27:N27"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="L29:P29"/>
@@ -2126,8 +2139,9 @@
     <mergeCell ref="C37:I37"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C35" r:id="rId1" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
-    <hyperlink ref="C37" r:id="rId2" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
+    <hyperlink ref="A27" r:id="rId1" display="https://groups.io/g/picoballoon/topic/110236980"/>
+    <hyperlink ref="C35" r:id="rId2" display="https://help.libreoffice.org/latest/en-US/text/scalc/guide/goalseek.html"/>
+    <hyperlink ref="C37" r:id="rId3" display="https://support.microsoft.com/en-us/office/use-goal-seek-to-find-the-result-you-want-by-adjusting-an-input-value-320cb99e-f4a4-417f-b1c3-4f369d6e66c7"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>